<commit_message>
actualizado schema das classes e relatorio.
</commit_message>
<xml_diff>
--- a/Relatório Projecto Final/Schemas/Classes/classesSchema.xlsx
+++ b/Relatório Projecto Final/Schemas/Classes/classesSchema.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silvia\ISEL\Repositorio Local\PDM\Relatório Projecto Final\Schemas\Classes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lima\ISEL\Ano 3\Semestre 5\PDM\repositorio\Relatório Projecto Final\Schemas\Classes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>SettingsActivity</t>
   </si>
@@ -33,12 +33,6 @@
   </si>
   <si>
     <t>Button - onClickListener</t>
-  </si>
-  <si>
-    <t>MainActivity</t>
-  </si>
-  <si>
-    <t>setOnClickListener</t>
   </si>
   <si>
     <t>ClassesCursorAdapter</t>
@@ -126,22 +120,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -185,53 +182,6 @@
         <a:xfrm flipH="1">
           <a:off x="1543050" y="590550"/>
           <a:ext cx="895350" cy="571500"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>102053</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="5" name="Straight Arrow Connector 4"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2544536" y="578304"/>
-          <a:ext cx="6803" cy="1353910"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -667,67 +617,63 @@
   <dimension ref="B2:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E3" sqref="E3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="I3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" s="3"/>
+      <c r="F3" s="4"/>
+      <c r="I3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="4"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
+      <c r="C4" s="2"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
     </row>
     <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="F7" s="2" t="s">
-        <v>5</v>
+      <c r="C7" s="4"/>
+      <c r="F7" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="G7" s="6"/>
-      <c r="H7" s="3"/>
+      <c r="H7" s="4"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="1"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
       <c r="H9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="3"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
     </row>
     <row r="12" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H12" s="3"/>
+      <c r="G12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>